<commit_message>
New commit: _ Input data update
</commit_message>
<xml_diff>
--- a/Input data/Input_data_reference.xlsx
+++ b/Input data/Input_data_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\PhD\Bottom-up &amp; scenarios\Modelling\Input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB35E76F-8440-4C2D-AE30-B4A0AA69159D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2F25F7-97A1-40E8-BF88-D9FEC4624BB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TECHNOLOGIES" sheetId="1" r:id="rId1"/>
@@ -3302,7 +3302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5648" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5650" uniqueCount="197">
   <si>
     <t>RESOURCES</t>
   </si>
@@ -4588,11 +4588,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E816912D-0BDF-41DD-ABBC-F7764F32EC0A}" name="Tableau4" displayName="Tableau4" ref="A1:F497" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:F497" xr:uid="{0228EFE9-A26D-47DE-80C5-467BC8C55473}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E816912D-0BDF-41DD-ABBC-F7764F32EC0A}" name="Tableau4" displayName="Tableau4" ref="A1:F498" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:F498" xr:uid="{0228EFE9-A26D-47DE-80C5-467BC8C55473}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Gasification"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="capacity_associated_resource"/>
+        <filter val="capex"/>
+        <filter val="flow_cost_t"/>
+        <filter val="opex_cost"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4640,9 +4647,14 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63D130C1-8AB1-4199-A675-E3E123196595}" name="Tableau1" displayName="Tableau1" ref="A1:F614" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:F614" xr:uid="{0BE97764-31A2-4AB2-B609-6BCFE43756E3}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Steel"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="emissions_r"/>
+        <filter val="output"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4985,10 +4997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J497"/>
+  <dimension ref="A1:J498"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F506" sqref="F506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5151,12 +5163,12 @@
         <v>546</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F14">
         <v>5443</v>
@@ -6375,7 +6387,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>68</v>
       </c>
@@ -6389,7 +6401,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>69</v>
       </c>
@@ -6403,7 +6415,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -6417,7 +6429,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>80</v>
       </c>
@@ -6431,7 +6443,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>81</v>
       </c>
@@ -6445,7 +6457,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>27</v>
       </c>
@@ -6456,7 +6468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>28</v>
       </c>
@@ -6467,7 +6479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>57</v>
       </c>
@@ -6481,7 +6493,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -6492,7 +6504,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>59</v>
       </c>
@@ -6503,7 +6515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -6514,7 +6526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>19</v>
       </c>
@@ -6525,7 +6537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>21</v>
       </c>
@@ -6536,7 +6548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>41</v>
       </c>
@@ -6547,7 +6559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>34</v>
       </c>
@@ -6558,7 +6570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>71</v>
       </c>
@@ -6572,7 +6584,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>72</v>
       </c>
@@ -6586,7 +6598,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>73</v>
       </c>
@@ -6600,7 +6612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>74</v>
       </c>
@@ -6614,7 +6626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>75</v>
       </c>
@@ -7188,7 +7200,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>27</v>
       </c>
@@ -7199,7 +7211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>28</v>
       </c>
@@ -7210,7 +7222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>57</v>
       </c>
@@ -7224,7 +7236,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>116</v>
       </c>
@@ -7235,7 +7247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>118</v>
       </c>
@@ -7246,7 +7258,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>119</v>
       </c>
@@ -7257,7 +7269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>120</v>
       </c>
@@ -7271,7 +7283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>121</v>
       </c>
@@ -8211,7 +8223,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>98</v>
       </c>
@@ -8225,7 +8237,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>100</v>
       </c>
@@ -8239,7 +8251,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>101</v>
       </c>
@@ -8253,7 +8265,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>102</v>
       </c>
@@ -8267,7 +8279,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>105</v>
       </c>
@@ -8281,7 +8293,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>106</v>
       </c>
@@ -8292,7 +8304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>107</v>
       </c>
@@ -8303,7 +8315,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>108</v>
       </c>
@@ -8314,7 +8326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>109</v>
       </c>
@@ -8325,7 +8337,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>132</v>
       </c>
@@ -8336,7 +8348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>133</v>
       </c>
@@ -8347,7 +8359,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>134</v>
       </c>
@@ -8358,7 +8370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>111</v>
       </c>
@@ -8369,7 +8381,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>112</v>
       </c>
@@ -8380,7 +8392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>113</v>
       </c>
@@ -8391,7 +8403,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>114</v>
       </c>
@@ -8933,7 +8945,7 @@
         <v>325000</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>138</v>
       </c>
@@ -8947,7 +8959,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>139</v>
       </c>
@@ -8961,7 +8973,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>140</v>
       </c>
@@ -8975,7 +8987,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>141</v>
       </c>
@@ -8989,7 +9001,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>142</v>
       </c>
@@ -10897,7 +10909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>146</v>
       </c>
@@ -10911,7 +10923,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>147</v>
       </c>
@@ -10925,7 +10937,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>163</v>
       </c>
@@ -10939,7 +10951,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>165</v>
       </c>
@@ -10953,7 +10965,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>157</v>
       </c>
@@ -10967,7 +10979,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>159</v>
       </c>
@@ -10981,7 +10993,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>161</v>
       </c>
@@ -10995,7 +11007,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>164</v>
       </c>
@@ -11009,7 +11021,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>166</v>
       </c>
@@ -11023,7 +11035,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>158</v>
       </c>
@@ -11037,7 +11049,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>160</v>
       </c>
@@ -11051,7 +11063,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>162</v>
       </c>
@@ -11065,7 +11077,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>176</v>
       </c>
@@ -11079,7 +11091,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>177</v>
       </c>
@@ -11093,7 +11105,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>174</v>
       </c>
@@ -11107,7 +11119,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>170</v>
       </c>
@@ -11121,7 +11133,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>171</v>
       </c>
@@ -11135,7 +11147,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>175</v>
       </c>
@@ -11149,7 +11161,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>172</v>
       </c>
@@ -11163,7 +11175,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>173</v>
       </c>
@@ -11177,7 +11189,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>149</v>
       </c>
@@ -11191,7 +11203,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>148</v>
       </c>
@@ -11712,7 +11724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>178</v>
       </c>
@@ -11726,7 +11738,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>179</v>
       </c>
@@ -12037,7 +12049,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>183</v>
       </c>
@@ -12090,7 +12102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>196</v>
       </c>
@@ -12146,7 +12158,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>186</v>
       </c>
@@ -12202,7 +12214,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>192</v>
       </c>
@@ -12258,7 +12270,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>194</v>
       </c>
@@ -12314,7 +12326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>195</v>
       </c>
@@ -12367,7 +12379,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>188</v>
       </c>
@@ -12420,7 +12432,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>193</v>
       </c>
@@ -12432,6 +12444,18 @@
       </c>
       <c r="F497" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>41</v>
+      </c>
+      <c r="E498" t="s">
+        <v>39</v>
+      </c>
+      <c r="F498">
+        <f>0.09*F14</f>
+        <v>489.87</v>
       </c>
     </row>
   </sheetData>
@@ -12448,8 +12472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14923,11 +14947,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AV126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="T38" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D79" sqref="D79"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18294,12 +18318,13 @@
   <dimension ref="A1:H614"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E217" sqref="E217"/>
+      <selection activeCell="E371" sqref="E371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22040,7 +22065,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>5</v>
       </c>
@@ -22051,7 +22076,7 @@
         <v>0.14360919999999999</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>6</v>
       </c>
@@ -22062,7 +22087,7 @@
         <v>-0.95</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>84</v>
       </c>
@@ -22073,7 +22098,7 @@
         <v>-0.378</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -22084,7 +22109,7 @@
         <v>0.66905599999999998</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -22095,7 +22120,7 @@
         <v>0.38638319999999998</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>11</v>
       </c>
@@ -22109,7 +22134,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>11</v>
       </c>
@@ -22123,7 +22148,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>11</v>
       </c>
@@ -22137,7 +22162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>8</v>
       </c>
@@ -22154,7 +22179,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>8</v>
       </c>
@@ -22171,7 +22196,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>8</v>
       </c>
@@ -22188,7 +22213,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>8</v>
       </c>
@@ -22205,7 +22230,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>8</v>
       </c>
@@ -22222,7 +22247,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>8</v>
       </c>
@@ -22239,7 +22264,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>8</v>
       </c>
@@ -22256,7 +22281,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>8</v>
       </c>
@@ -22273,7 +22298,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>8</v>
       </c>
@@ -22290,7 +22315,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>8</v>
       </c>
@@ -22307,7 +22332,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>8</v>
       </c>
@@ -22324,7 +22349,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>8</v>
       </c>
@@ -22341,7 +22366,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>8</v>
       </c>
@@ -22355,7 +22380,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>26</v>
       </c>
@@ -22366,7 +22391,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>54</v>
       </c>
@@ -22377,7 +22402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>53</v>
       </c>
@@ -24746,7 +24771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>12</v>
       </c>
@@ -24766,7 +24791,7 @@
         <v>9800000</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>17</v>
       </c>
@@ -24786,7 +24811,7 @@
         <v>5200000</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>12</v>
       </c>
@@ -24806,7 +24831,7 @@
         <v>9800000</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>17</v>
       </c>
@@ -24868,7 +24893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>12</v>
       </c>
@@ -24888,7 +24913,7 @@
         <v>9800000</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>17</v>
       </c>
@@ -24908,7 +24933,7 @@
         <v>5200000</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>12</v>
       </c>
@@ -24928,7 +24953,7 @@
         <v>8650000</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>17</v>
       </c>
@@ -24948,7 +24973,7 @@
         <v>6350000</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>12</v>
       </c>
@@ -24968,7 +24993,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>17</v>
       </c>
@@ -24988,7 +25013,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>12</v>
       </c>
@@ -25008,7 +25033,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>17</v>
       </c>
@@ -25028,7 +25053,7 @@
         <v>12600000</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>12</v>
       </c>
@@ -25048,7 +25073,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>17</v>
       </c>
@@ -25068,7 +25093,7 @@
         <v>12600000</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>12</v>
       </c>
@@ -25088,7 +25113,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>17</v>
       </c>
@@ -25108,7 +25133,7 @@
         <v>12600000</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>12</v>
       </c>
@@ -25128,7 +25153,7 @@
         <v>25650000</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>17</v>
       </c>
@@ -25148,7 +25173,7 @@
         <v>16950000</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>12</v>
       </c>
@@ -25168,7 +25193,7 @@
         <v>21300000</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>17</v>
       </c>
@@ -25188,7 +25213,7 @@
         <v>21300000</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>12</v>
       </c>
@@ -25208,7 +25233,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>17</v>
       </c>
@@ -25228,7 +25253,7 @@
         <v>17200000</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>12</v>
       </c>
@@ -25248,7 +25273,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>17</v>
       </c>
@@ -25268,7 +25293,7 @@
         <v>17200000</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>12</v>
       </c>
@@ -25288,7 +25313,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>17</v>
       </c>
@@ -25308,7 +25333,7 @@
         <v>17200000</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>12</v>
       </c>
@@ -25328,7 +25353,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>17</v>
       </c>
@@ -25348,7 +25373,7 @@
         <v>17200000</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>12</v>
       </c>
@@ -25368,7 +25393,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>17</v>
       </c>
@@ -25388,7 +25413,7 @@
         <v>17200000</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>12</v>
       </c>
@@ -25408,7 +25433,7 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>17</v>
       </c>
@@ -25428,7 +25453,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>12</v>
       </c>
@@ -25448,7 +25473,7 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>17</v>
       </c>
@@ -25468,7 +25493,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>12</v>
       </c>
@@ -25488,7 +25513,7 @@
         <v>9000000</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>17</v>
       </c>
@@ -25508,7 +25533,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>12</v>
       </c>
@@ -25528,7 +25553,7 @@
         <v>7250000</v>
       </c>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>17</v>
       </c>
@@ -25548,7 +25573,7 @@
         <v>3750000</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>12</v>
       </c>
@@ -25568,7 +25593,7 @@
         <v>5500000</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>17</v>
       </c>
@@ -25588,7 +25613,7 @@
         <v>5500000</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>12</v>
       </c>
@@ -25608,7 +25633,7 @@
         <v>4700000</v>
       </c>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>17</v>
       </c>
@@ -25628,7 +25653,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>12</v>
       </c>
@@ -25648,7 +25673,7 @@
         <v>4700000</v>
       </c>
     </row>
-    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>17</v>
       </c>
@@ -25668,7 +25693,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>12</v>
       </c>
@@ -25688,7 +25713,7 @@
         <v>4700000</v>
       </c>
     </row>
-    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>17</v>
       </c>
@@ -25708,7 +25733,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>12</v>
       </c>
@@ -25728,7 +25753,7 @@
         <v>4700000</v>
       </c>
     </row>
-    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>17</v>
       </c>
@@ -25748,7 +25773,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>12</v>
       </c>
@@ -25768,7 +25793,7 @@
         <v>4700000</v>
       </c>
     </row>
-    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>17</v>
       </c>
@@ -25788,7 +25813,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>12</v>
       </c>
@@ -25808,7 +25833,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>17</v>
       </c>
@@ -25828,7 +25853,7 @@
         <v>2400000</v>
       </c>
     </row>
-    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>12</v>
       </c>
@@ -25848,7 +25873,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>17</v>
       </c>
@@ -25868,7 +25893,7 @@
         <v>2400000</v>
       </c>
     </row>
-    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>12</v>
       </c>
@@ -25888,7 +25913,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>17</v>
       </c>
@@ -25908,7 +25933,7 @@
         <v>2400000</v>
       </c>
     </row>
-    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>12</v>
       </c>
@@ -25928,7 +25953,7 @@
         <v>4199999.9999999991</v>
       </c>
     </row>
-    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>17</v>
       </c>
@@ -25948,7 +25973,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>12</v>
       </c>
@@ -25968,7 +25993,7 @@
         <v>3599999.9999999995</v>
       </c>
     </row>
-    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>17</v>
       </c>

</xml_diff>